<commit_message>
Add task position selection popup and update styles
</commit_message>
<xml_diff>
--- a/Task-list-Aeon.xlsx
+++ b/Task-list-Aeon.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\auraProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305"/>
+    <workbookView minimized="1" xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305"/>
   </bookViews>
   <sheets>
     <sheet name="Rule-Task list" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Rule-Task list'!$A$1:$J$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -320,7 +320,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -938,7 +938,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P3" sqref="P3"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,19 +1745,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
     <mergeCell ref="E20:J20"/>
     <mergeCell ref="E21:J21"/>
     <mergeCell ref="E22:J22"/>
@@ -1768,6 +1755,19 @@
     <mergeCell ref="E17:J17"/>
     <mergeCell ref="E18:J18"/>
     <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>